<commit_message>
erster Erfolgreicher Import von MA
</commit_message>
<xml_diff>
--- a/testdaten/Firma1/Mitarbeiterliste_120_Personen.xlsx
+++ b/testdaten/Firma1/Mitarbeiterliste_120_Personen.xlsx
@@ -1,22 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git_d12\MitbestimmIT\testdaten\Firma1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9933573-CACF-470D-A858-51C8DC9693FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E568A38-B6A3-4F9C-99B9-1D4710C63F6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5025" yWindow="5025" windowWidth="38700" windowHeight="15345" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19860" yWindow="5490" windowWidth="38700" windowHeight="15345" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -25,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="364">
   <si>
     <t>Personalnummer</t>
   </si>
@@ -754,6 +765,369 @@
   </si>
   <si>
     <t>Beerdigungen</t>
+  </si>
+  <si>
+    <t>GebDat</t>
+  </si>
+  <si>
+    <t>22.06.1988</t>
+  </si>
+  <si>
+    <t>11.05.1983</t>
+  </si>
+  <si>
+    <t>28.11.1995</t>
+  </si>
+  <si>
+    <t>05.06.1983</t>
+  </si>
+  <si>
+    <t>02.03.1985</t>
+  </si>
+  <si>
+    <t>31.05.1990</t>
+  </si>
+  <si>
+    <t>28.06.1984</t>
+  </si>
+  <si>
+    <t>14.12.1984</t>
+  </si>
+  <si>
+    <t>14.02.1988</t>
+  </si>
+  <si>
+    <t>08.05.1988</t>
+  </si>
+  <si>
+    <t>21.02.1980</t>
+  </si>
+  <si>
+    <t>01.10.1987</t>
+  </si>
+  <si>
+    <t>26.02.1993</t>
+  </si>
+  <si>
+    <t>14.02.1987</t>
+  </si>
+  <si>
+    <t>03.06.1990</t>
+  </si>
+  <si>
+    <t>31.05.1989</t>
+  </si>
+  <si>
+    <t>17.08.1994</t>
+  </si>
+  <si>
+    <t>16.10.1989</t>
+  </si>
+  <si>
+    <t>16.08.1982</t>
+  </si>
+  <si>
+    <t>01.01.1988</t>
+  </si>
+  <si>
+    <t>01.01.1986</t>
+  </si>
+  <si>
+    <t>07.11.1985</t>
+  </si>
+  <si>
+    <t>03.07.1980</t>
+  </si>
+  <si>
+    <t>24.04.1996</t>
+  </si>
+  <si>
+    <t>18.01.1985</t>
+  </si>
+  <si>
+    <t>21.03.1988</t>
+  </si>
+  <si>
+    <t>14.11.1980</t>
+  </si>
+  <si>
+    <t>01.01.1980</t>
+  </si>
+  <si>
+    <t>14.09.1985</t>
+  </si>
+  <si>
+    <t>23.09.1985</t>
+  </si>
+  <si>
+    <t>10.02.1996</t>
+  </si>
+  <si>
+    <t>28.09.1984</t>
+  </si>
+  <si>
+    <t>25.03.1989</t>
+  </si>
+  <si>
+    <t>01.06.1989</t>
+  </si>
+  <si>
+    <t>18.03.1984</t>
+  </si>
+  <si>
+    <t>10.05.1983</t>
+  </si>
+  <si>
+    <t>15.07.1988</t>
+  </si>
+  <si>
+    <t>20.01.1989</t>
+  </si>
+  <si>
+    <t>28.07.1997</t>
+  </si>
+  <si>
+    <t>10.09.1996</t>
+  </si>
+  <si>
+    <t>23.05.1982</t>
+  </si>
+  <si>
+    <t>12.10.1983</t>
+  </si>
+  <si>
+    <t>29.09.1984</t>
+  </si>
+  <si>
+    <t>12.12.1999</t>
+  </si>
+  <si>
+    <t>21.11.1992</t>
+  </si>
+  <si>
+    <t>21.09.1989</t>
+  </si>
+  <si>
+    <t>13.12.1984</t>
+  </si>
+  <si>
+    <t>11.08.1988</t>
+  </si>
+  <si>
+    <t>03.10.1983</t>
+  </si>
+  <si>
+    <t>24.09.1998</t>
+  </si>
+  <si>
+    <t>13.02.1985</t>
+  </si>
+  <si>
+    <t>01.05.1990</t>
+  </si>
+  <si>
+    <t>13.02.1986</t>
+  </si>
+  <si>
+    <t>12.05.1999</t>
+  </si>
+  <si>
+    <t>18.02.1981</t>
+  </si>
+  <si>
+    <t>30.12.1991</t>
+  </si>
+  <si>
+    <t>20.11.1993</t>
+  </si>
+  <si>
+    <t>28.03.1988</t>
+  </si>
+  <si>
+    <t>11.08.1997</t>
+  </si>
+  <si>
+    <t>10.09.1980</t>
+  </si>
+  <si>
+    <t>13.03.1996</t>
+  </si>
+  <si>
+    <t>29.01.1988</t>
+  </si>
+  <si>
+    <t>21.11.1989</t>
+  </si>
+  <si>
+    <t>10.03.1992</t>
+  </si>
+  <si>
+    <t>11.05.1997</t>
+  </si>
+  <si>
+    <t>15.02.1997</t>
+  </si>
+  <si>
+    <t>03.07.1987</t>
+  </si>
+  <si>
+    <t>14.06.1997</t>
+  </si>
+  <si>
+    <t>10.06.1989</t>
+  </si>
+  <si>
+    <t>12.02.1982</t>
+  </si>
+  <si>
+    <t>02.05.1984</t>
+  </si>
+  <si>
+    <t>01.07.1984</t>
+  </si>
+  <si>
+    <t>20.07.1986</t>
+  </si>
+  <si>
+    <t>18.05.1995</t>
+  </si>
+  <si>
+    <t>30.06.1988</t>
+  </si>
+  <si>
+    <t>17.02.1990</t>
+  </si>
+  <si>
+    <t>01.05.1988</t>
+  </si>
+  <si>
+    <t>09.12.1999</t>
+  </si>
+  <si>
+    <t>13.09.1983</t>
+  </si>
+  <si>
+    <t>19.06.2000</t>
+  </si>
+  <si>
+    <t>16.08.1996</t>
+  </si>
+  <si>
+    <t>24.06.1997</t>
+  </si>
+  <si>
+    <t>05.11.2000</t>
+  </si>
+  <si>
+    <t>04.02.1995</t>
+  </si>
+  <si>
+    <t>27.06.1987</t>
+  </si>
+  <si>
+    <t>21.10.1988</t>
+  </si>
+  <si>
+    <t>20.03.1988</t>
+  </si>
+  <si>
+    <t>13.07.1981</t>
+  </si>
+  <si>
+    <t>25.01.1983</t>
+  </si>
+  <si>
+    <t>15.08.2000</t>
+  </si>
+  <si>
+    <t>28.11.1989</t>
+  </si>
+  <si>
+    <t>27.05.1994</t>
+  </si>
+  <si>
+    <t>20.11.1997</t>
+  </si>
+  <si>
+    <t>30.12.1985</t>
+  </si>
+  <si>
+    <t>30.07.1984</t>
+  </si>
+  <si>
+    <t>19.08.1995</t>
+  </si>
+  <si>
+    <t>09.05.1995</t>
+  </si>
+  <si>
+    <t>24.02.1986</t>
+  </si>
+  <si>
+    <t>15.01.1993</t>
+  </si>
+  <si>
+    <t>11.04.1988</t>
+  </si>
+  <si>
+    <t>20.10.1983</t>
+  </si>
+  <si>
+    <t>03.10.1991</t>
+  </si>
+  <si>
+    <t>30.08.1983</t>
+  </si>
+  <si>
+    <t>23.07.1982</t>
+  </si>
+  <si>
+    <t>01.12.1997</t>
+  </si>
+  <si>
+    <t>01.06.1983</t>
+  </si>
+  <si>
+    <t>20.08.1987</t>
+  </si>
+  <si>
+    <t>26.05.1999</t>
+  </si>
+  <si>
+    <t>07.04.1981</t>
+  </si>
+  <si>
+    <t>22.08.1993</t>
+  </si>
+  <si>
+    <t>16.08.1983</t>
+  </si>
+  <si>
+    <t>02.08.1983</t>
+  </si>
+  <si>
+    <t>19.02.1996</t>
+  </si>
+  <si>
+    <t>20.06.1993</t>
+  </si>
+  <si>
+    <t>25.10.1981</t>
+  </si>
+  <si>
+    <t>12.06.1986</t>
+  </si>
+  <si>
+    <t>09.07.1993</t>
+  </si>
+  <si>
+    <t>26.10.1995</t>
+  </si>
+  <si>
+    <t>09.03.1996</t>
+  </si>
+  <si>
+    <t>24.07.1996</t>
   </si>
 </sst>
 </file>
@@ -791,7 +1165,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -814,11 +1188,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -833,6 +1218,9 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1032,7 +1420,7 @@
   <dimension ref="A1:F122"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1042,6 +1430,7 @@
     <col min="3" max="3" width="13.7109375" customWidth="1"/>
     <col min="4" max="4" width="11.140625" customWidth="1"/>
     <col min="5" max="5" width="22.7109375" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -1060,6 +1449,9 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="6" t="s">
+        <v>243</v>
+      </c>
     </row>
     <row r="2" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
@@ -1077,7 +1469,9 @@
       <c r="E2" s="3" t="s">
         <v>242</v>
       </c>
-      <c r="F2" s="4"/>
+      <c r="F2" s="4" t="s">
+        <v>249</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -1095,6 +1489,9 @@
       <c r="E3" t="s">
         <v>8</v>
       </c>
+      <c r="F3" s="4" t="s">
+        <v>250</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -1112,6 +1509,9 @@
       <c r="E4" t="s">
         <v>10</v>
       </c>
+      <c r="F4" s="4" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -1129,6 +1529,9 @@
       <c r="E5" t="s">
         <v>13</v>
       </c>
+      <c r="F5" s="4" t="s">
+        <v>252</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -1146,6 +1549,9 @@
       <c r="E6" t="s">
         <v>8</v>
       </c>
+      <c r="F6" s="4" t="s">
+        <v>253</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -1163,6 +1569,9 @@
       <c r="E7" t="s">
         <v>19</v>
       </c>
+      <c r="F7" s="4" t="s">
+        <v>254</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -1180,6 +1589,9 @@
       <c r="E8" t="s">
         <v>22</v>
       </c>
+      <c r="F8" s="4" t="s">
+        <v>255</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -1197,6 +1609,9 @@
       <c r="E9" t="s">
         <v>22</v>
       </c>
+      <c r="F9" s="4" t="s">
+        <v>247</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -1214,6 +1629,9 @@
       <c r="E10" t="s">
         <v>10</v>
       </c>
+      <c r="F10" s="4" t="s">
+        <v>256</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -1231,6 +1649,9 @@
       <c r="E11" t="s">
         <v>10</v>
       </c>
+      <c r="F11" s="4" t="s">
+        <v>248</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -1248,6 +1669,9 @@
       <c r="E12" t="s">
         <v>31</v>
       </c>
+      <c r="F12" s="4" t="s">
+        <v>245</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
@@ -1265,6 +1689,9 @@
       <c r="E13" t="s">
         <v>22</v>
       </c>
+      <c r="F13" s="4" t="s">
+        <v>257</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -1282,6 +1709,9 @@
       <c r="E14" t="s">
         <v>10</v>
       </c>
+      <c r="F14" s="4" t="s">
+        <v>258</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
@@ -1299,6 +1729,9 @@
       <c r="E15" t="s">
         <v>31</v>
       </c>
+      <c r="F15" s="4" t="s">
+        <v>259</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
@@ -1316,8 +1749,11 @@
       <c r="E16" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F16" s="4" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>105075</v>
       </c>
@@ -1333,8 +1769,11 @@
       <c r="E17" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F17" s="4" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>105076</v>
       </c>
@@ -1350,8 +1789,11 @@
       <c r="E18" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F18" s="4" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>105077</v>
       </c>
@@ -1367,8 +1809,11 @@
       <c r="E19" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F19" s="4" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>105078</v>
       </c>
@@ -1384,8 +1829,11 @@
       <c r="E20" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F20" s="4" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>105079</v>
       </c>
@@ -1401,8 +1849,11 @@
       <c r="E21" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F21" s="4" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>105080</v>
       </c>
@@ -1418,8 +1869,11 @@
       <c r="E22" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F22" s="4" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>105081</v>
       </c>
@@ -1435,8 +1889,11 @@
       <c r="E23" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F23" s="4" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>105082</v>
       </c>
@@ -1452,8 +1909,11 @@
       <c r="E24" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F24" s="4" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>105083</v>
       </c>
@@ -1469,8 +1929,11 @@
       <c r="E25" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F25" s="4" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>105084</v>
       </c>
@@ -1486,8 +1949,11 @@
       <c r="E26" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F26" s="4" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>105085</v>
       </c>
@@ -1503,8 +1969,11 @@
       <c r="E27" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F27" s="4" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>105086</v>
       </c>
@@ -1520,8 +1989,11 @@
       <c r="E28" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F28" s="4" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>105087</v>
       </c>
@@ -1537,8 +2009,11 @@
       <c r="E29" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F29" s="4" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>105088</v>
       </c>
@@ -1554,8 +2029,11 @@
       <c r="E30" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F30" s="4" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>105089</v>
       </c>
@@ -1571,8 +2049,11 @@
       <c r="E31" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F31" s="4" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>105090</v>
       </c>
@@ -1588,8 +2069,11 @@
       <c r="E32" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F32" s="4" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>105091</v>
       </c>
@@ -1605,8 +2089,11 @@
       <c r="E33" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F33" s="4" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>105092</v>
       </c>
@@ -1622,8 +2109,11 @@
       <c r="E34" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F34" s="4" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>105093</v>
       </c>
@@ -1639,8 +2129,11 @@
       <c r="E35" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F35" s="4" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>105094</v>
       </c>
@@ -1656,8 +2149,11 @@
       <c r="E36" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F36" s="4" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>105095</v>
       </c>
@@ -1673,8 +2169,11 @@
       <c r="E37" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F37" s="4" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>105096</v>
       </c>
@@ -1690,8 +2189,11 @@
       <c r="E38" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F38" s="4" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>105097</v>
       </c>
@@ -1707,8 +2209,11 @@
       <c r="E39" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F39" s="4" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>105098</v>
       </c>
@@ -1724,8 +2229,11 @@
       <c r="E40" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F40" s="4" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>105099</v>
       </c>
@@ -1741,8 +2249,11 @@
       <c r="E41" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F41" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>105100</v>
       </c>
@@ -1758,8 +2269,11 @@
       <c r="E42" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F42" s="4" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>105101</v>
       </c>
@@ -1775,8 +2289,11 @@
       <c r="E43" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F43" s="4" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>105102</v>
       </c>
@@ -1792,8 +2309,11 @@
       <c r="E44" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F44" s="4" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>105103</v>
       </c>
@@ -1809,8 +2329,11 @@
       <c r="E45" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F45" s="4" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>105104</v>
       </c>
@@ -1826,8 +2349,11 @@
       <c r="E46" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F46" s="4" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>105105</v>
       </c>
@@ -1843,8 +2369,11 @@
       <c r="E47" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F47" s="4" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>105106</v>
       </c>
@@ -1860,8 +2389,11 @@
       <c r="E48" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F48" s="4" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>105107</v>
       </c>
@@ -1877,8 +2409,11 @@
       <c r="E49" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F49" s="4" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>105108</v>
       </c>
@@ -1894,8 +2429,11 @@
       <c r="E50" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F50" s="4" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>105109</v>
       </c>
@@ -1911,8 +2449,11 @@
       <c r="E51" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F51" s="4" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>105110</v>
       </c>
@@ -1928,8 +2469,11 @@
       <c r="E52" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F52" s="4" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>105111</v>
       </c>
@@ -1945,8 +2489,11 @@
       <c r="E53" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F53" s="4" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>105112</v>
       </c>
@@ -1962,8 +2509,11 @@
       <c r="E54" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F54" s="4" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>105113</v>
       </c>
@@ -1979,8 +2529,11 @@
       <c r="E55" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F55" s="4" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>105114</v>
       </c>
@@ -1996,8 +2549,11 @@
       <c r="E56" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F56" s="4" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>105115</v>
       </c>
@@ -2013,8 +2569,11 @@
       <c r="E57" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F57" s="4" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>105116</v>
       </c>
@@ -2030,8 +2589,11 @@
       <c r="E58" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F58" s="4" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>105117</v>
       </c>
@@ -2047,8 +2609,11 @@
       <c r="E59" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F59" s="4" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>105118</v>
       </c>
@@ -2064,8 +2629,11 @@
       <c r="E60" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F60" s="4" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>105119</v>
       </c>
@@ -2081,8 +2649,11 @@
       <c r="E61" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F61" s="4" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>105120</v>
       </c>
@@ -2098,8 +2669,11 @@
       <c r="E62" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F62" s="4" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>105121</v>
       </c>
@@ -2115,8 +2689,11 @@
       <c r="E63" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F63" s="4" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>105122</v>
       </c>
@@ -2132,8 +2709,11 @@
       <c r="E64" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F64" s="4" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>105123</v>
       </c>
@@ -2149,8 +2729,11 @@
       <c r="E65" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F65" s="4" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>105124</v>
       </c>
@@ -2166,8 +2749,11 @@
       <c r="E66" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F66" s="4" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>105125</v>
       </c>
@@ -2183,8 +2769,11 @@
       <c r="E67" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F67" s="4" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>105126</v>
       </c>
@@ -2200,8 +2789,11 @@
       <c r="E68" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F68" s="4" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>105127</v>
       </c>
@@ -2217,8 +2809,11 @@
       <c r="E69" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F69" s="4" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>105128</v>
       </c>
@@ -2234,8 +2829,11 @@
       <c r="E70" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F70" s="4" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>105129</v>
       </c>
@@ -2251,8 +2849,11 @@
       <c r="E71" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F71" s="4" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>105130</v>
       </c>
@@ -2268,8 +2869,11 @@
       <c r="E72" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F72" s="4" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>105131</v>
       </c>
@@ -2285,8 +2889,11 @@
       <c r="E73" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F73" s="4" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>105132</v>
       </c>
@@ -2302,8 +2909,11 @@
       <c r="E74" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F74" s="4" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>105133</v>
       </c>
@@ -2319,8 +2929,11 @@
       <c r="E75" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F75" s="4" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>105134</v>
       </c>
@@ -2336,8 +2949,11 @@
       <c r="E76" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F76" s="4" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>105135</v>
       </c>
@@ -2353,8 +2969,11 @@
       <c r="E77" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F77" s="4" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>105136</v>
       </c>
@@ -2370,8 +2989,11 @@
       <c r="E78" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F78" s="4" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>105137</v>
       </c>
@@ -2387,8 +3009,11 @@
       <c r="E79" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F79" s="4" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>105138</v>
       </c>
@@ -2404,8 +3029,11 @@
       <c r="E80" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F80" s="4" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>105139</v>
       </c>
@@ -2421,8 +3049,11 @@
       <c r="E81" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F81" s="4" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>105140</v>
       </c>
@@ -2438,8 +3069,11 @@
       <c r="E82" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F82" s="4" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>105141</v>
       </c>
@@ -2455,8 +3089,11 @@
       <c r="E83" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F83" s="4" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>105142</v>
       </c>
@@ -2472,8 +3109,11 @@
       <c r="E84" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F84" s="4" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>105143</v>
       </c>
@@ -2489,8 +3129,11 @@
       <c r="E85" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F85" s="4" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>105144</v>
       </c>
@@ -2506,8 +3149,11 @@
       <c r="E86" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F86" s="4" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>105145</v>
       </c>
@@ -2523,8 +3169,11 @@
       <c r="E87" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F87" s="4" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>105146</v>
       </c>
@@ -2540,8 +3189,11 @@
       <c r="E88" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F88" s="4" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>105147</v>
       </c>
@@ -2557,8 +3209,11 @@
       <c r="E89" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F89" s="4" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>105148</v>
       </c>
@@ -2574,8 +3229,11 @@
       <c r="E90" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F90" s="4" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>105149</v>
       </c>
@@ -2591,8 +3249,11 @@
       <c r="E91" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F91" s="4" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>105150</v>
       </c>
@@ -2608,8 +3269,11 @@
       <c r="E92" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F92" s="4" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>105151</v>
       </c>
@@ -2625,8 +3289,11 @@
       <c r="E93" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F93" s="4" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>105152</v>
       </c>
@@ -2642,8 +3309,11 @@
       <c r="E94" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F94" s="4" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>105153</v>
       </c>
@@ -2659,8 +3329,11 @@
       <c r="E95" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F95" s="4" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>105154</v>
       </c>
@@ -2676,8 +3349,11 @@
       <c r="E96" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F96" s="4" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>105155</v>
       </c>
@@ -2693,8 +3369,11 @@
       <c r="E97" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F97" s="4" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>105156</v>
       </c>
@@ -2710,8 +3389,11 @@
       <c r="E98" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F98" s="4" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>105157</v>
       </c>
@@ -2727,8 +3409,11 @@
       <c r="E99" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F99" s="4" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>105158</v>
       </c>
@@ -2744,8 +3429,11 @@
       <c r="E100" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F100" s="4" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>105159</v>
       </c>
@@ -2761,8 +3449,11 @@
       <c r="E101" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F101" s="4" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>105160</v>
       </c>
@@ -2778,8 +3469,11 @@
       <c r="E102" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F102" s="4" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>105161</v>
       </c>
@@ -2795,8 +3489,11 @@
       <c r="E103" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F103" s="4" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>105162</v>
       </c>
@@ -2812,8 +3509,11 @@
       <c r="E104" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F104" s="4" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>105163</v>
       </c>
@@ -2829,8 +3529,11 @@
       <c r="E105" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F105" s="4" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>105164</v>
       </c>
@@ -2846,8 +3549,11 @@
       <c r="E106" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F106" s="4" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>105165</v>
       </c>
@@ -2863,8 +3569,11 @@
       <c r="E107" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F107" s="4" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>105166</v>
       </c>
@@ -2880,8 +3589,11 @@
       <c r="E108" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F108" s="4" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>105167</v>
       </c>
@@ -2897,8 +3609,11 @@
       <c r="E109" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F109" s="4" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>105168</v>
       </c>
@@ -2914,8 +3629,11 @@
       <c r="E110" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F110" s="4" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>105169</v>
       </c>
@@ -2931,8 +3649,11 @@
       <c r="E111" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F111" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>105170</v>
       </c>
@@ -2948,8 +3669,11 @@
       <c r="E112" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F112" s="4" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>105171</v>
       </c>
@@ -2965,8 +3689,11 @@
       <c r="E113" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F113" s="4" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>105172</v>
       </c>
@@ -2982,8 +3709,11 @@
       <c r="E114" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F114" s="4" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>105173</v>
       </c>
@@ -2999,8 +3729,11 @@
       <c r="E115" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F115" s="4" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>105174</v>
       </c>
@@ -3016,8 +3749,11 @@
       <c r="E116" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F116" s="4" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>105175</v>
       </c>
@@ -3033,8 +3769,11 @@
       <c r="E117" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F117" s="4" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>105176</v>
       </c>
@@ -3050,8 +3789,11 @@
       <c r="E118" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F118" s="4" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>105177</v>
       </c>
@@ -3067,8 +3809,11 @@
       <c r="E119" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F119" s="4" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>105178</v>
       </c>
@@ -3084,8 +3829,11 @@
       <c r="E120" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F120" s="4" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>105179</v>
       </c>
@@ -3101,8 +3849,11 @@
       <c r="E121" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F121" s="4" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>105180</v>
       </c>
@@ -3117,6 +3868,9 @@
       </c>
       <c r="E122" t="s">
         <v>22</v>
+      </c>
+      <c r="F122" s="4" t="s">
+        <v>363</v>
       </c>
     </row>
   </sheetData>

</xml_diff>